<commit_message>
Add adjustments and bug fixes to the formatters. Add formatters unit tests specification and implementation.
</commit_message>
<xml_diff>
--- a/docs/test cases/formatter/FastaFormatterTests.xlsx
+++ b/docs/test cases/formatter/FastaFormatterTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto\PhyloDB\docs\test cases\formatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92097D2-3EB7-4CD9-9998-F68AF36B3C26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D526DD9A-7423-4AF8-80BE-E584721BDF4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Parameter</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Choices</t>
   </si>
   <si>
-    <t>Valid</t>
-  </si>
-  <si>
     <t>Special Cases</t>
   </si>
   <si>
@@ -51,52 +48,82 @@
     <t>Output</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>dataset</t>
-  </si>
-  <si>
     <t>parse</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>null, empty, singleton</t>
-  </si>
-  <si>
-    <t>Dataset, null</t>
-  </si>
-  <si>
     <t>n = some &gt; 1</t>
   </si>
   <si>
-    <t>null, empty, singleton, invalid format</t>
-  </si>
-  <si>
     <t>empty</t>
   </si>
   <si>
-    <t>singleton</t>
-  </si>
-  <si>
-    <t>invalid format</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
-    <t>String(FASTA)</t>
-  </si>
-  <si>
-    <t>String, null</t>
-  </si>
-  <si>
-    <t>n size</t>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>n-elements</t>
+  </si>
+  <si>
+    <t>0, 1</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>profiles</t>
+  </si>
+  <si>
+    <t>list with n size</t>
+  </si>
+  <si>
+    <t>emptylist, singletonlist</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>nlist</t>
+  </si>
+  <si>
+    <t>emptylist</t>
+  </si>
+  <si>
+    <t>singletonlist</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>alleles</t>
+  </si>
+  <si>
+    <t>alfanumerical chars(ACTG)</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>fileAlleles</t>
+  </si>
+  <si>
+    <t>ACTG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlist - nothers </t>
+  </si>
+  <si>
+    <t>0(empty)</t>
+  </si>
+  <si>
+    <t>1(lines before id)</t>
+  </si>
+  <si>
+    <t>0(lines)</t>
   </si>
 </sst>
 </file>
@@ -128,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,14 +212,29 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,23 +242,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,31 +555,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -534,257 +591,328 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
+      <c r="A5" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>5</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>2</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>3</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>4</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A17:A18"/>
+  <mergeCells count="7">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>